<commit_message>
C. necator first draft full worked through
</commit_message>
<xml_diff>
--- a/docs/examples/Literature data/Cupriavidus necator  Alagesan 2017/estimated fluxes.xlsx
+++ b/docs/examples/Literature data/Cupriavidus necator  Alagesan 2017/estimated fluxes.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s143838/projects/AutoFlow-OmicsDataHandling/docs/examples/Literature data/Cupriavidus necator  Alagesan 2017/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6939BBBF-F404-E140-8A58-7D4560CAE28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26700" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="OLE_LINK1" localSheetId="0">'Ark1'!$A$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -18,12 +27,175 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+  <si>
+    <t>s.no</t>
+  </si>
+  <si>
+    <t>Reactions</t>
+  </si>
+  <si>
+    <t>Hetero-Fructose</t>
+  </si>
+  <si>
+    <t>Hetero- glycerol</t>
+  </si>
+  <si>
+    <t>Mixo-glycerol</t>
+  </si>
+  <si>
+    <t>(0.90,1.08)</t>
+  </si>
+  <si>
+    <t>(-1.05, -0.94)</t>
+  </si>
+  <si>
+    <t>(-5.84,-5.08)</t>
+  </si>
+  <si>
+    <t>(0.80, 0.96)</t>
+  </si>
+  <si>
+    <t>(-0.3,-0.06)</t>
+  </si>
+  <si>
+    <t>(-0.03,0.0)</t>
+  </si>
+  <si>
+    <t>(0.38,0.50)</t>
+  </si>
+  <si>
+    <t>(0.009, 0.15)</t>
+  </si>
+  <si>
+    <t>(1.09,1.3)</t>
+  </si>
+  <si>
+    <t>(0.39, 0.6)</t>
+  </si>
+  <si>
+    <t>(0.01,0.04)</t>
+  </si>
+  <si>
+    <t>(0.9,1.1)</t>
+  </si>
+  <si>
+    <t>(0.38,0.45)</t>
+  </si>
+  <si>
+    <t>(0.007,0.01)</t>
+  </si>
+  <si>
+    <t>(0.75, 1.0)</t>
+  </si>
+  <si>
+    <t>(0.96,1.27)</t>
+  </si>
+  <si>
+    <t>(0.87,0.96)</t>
+  </si>
+  <si>
+    <t>(1.71,2.13)</t>
+  </si>
+  <si>
+    <t>(0.0,0.0)</t>
+  </si>
+  <si>
+    <t>(0.0,0.001)</t>
+  </si>
+  <si>
+    <t>(0.22,0.32)</t>
+  </si>
+  <si>
+    <t>(1.26, 2.36)</t>
+  </si>
+  <si>
+    <t>(0.001,0.09)</t>
+  </si>
+  <si>
+    <t>(0.88,1.01)</t>
+  </si>
+  <si>
+    <t>(1.18,2.77)</t>
+  </si>
+  <si>
+    <t>(0.0,0.003)</t>
+  </si>
+  <si>
+    <t>(0.27,0.44)</t>
+  </si>
+  <si>
+    <t>(0.0,0.03)</t>
+  </si>
+  <si>
+    <t>(0.32,0.35)</t>
+  </si>
+  <si>
+    <t>(0.9, 0.99)</t>
+  </si>
+  <si>
+    <t>(0.2, 0.44)</t>
+  </si>
+  <si>
+    <t>(2.7, 2.96)</t>
+  </si>
+  <si>
+    <t>G3P &lt;-&gt; 3PG</t>
+  </si>
+  <si>
+    <t>3PG &lt;-&gt; PEP</t>
+  </si>
+  <si>
+    <t>PYR -&gt; ACCOA + CO2</t>
+  </si>
+  <si>
+    <t>OAA + ACCOA -&gt; CIT</t>
+  </si>
+  <si>
+    <t>ISCIT -&gt; AKG + CO2</t>
+  </si>
+  <si>
+    <t>6PG -&gt; PYR + G3P</t>
+  </si>
+  <si>
+    <t>ISCIT -&gt; GLYOXY + 0.5 SUC + 0.5 SUC</t>
+  </si>
+  <si>
+    <t>PEP + CO2 &lt;-&gt; OAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OAA -&gt; PYR + CO2  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F6P + G3P &lt;-&gt; E4P + X5P </t>
+  </si>
+  <si>
+    <t>RUBP + CO2 -&gt; 3PG + 3PG</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -37,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,12 +217,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +569,220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>